<commit_message>
shope bacis function finished
</commit_message>
<xml_diff>
--- a/src/electron/crawler/config/output.xlsx
+++ b/src/electron/crawler/config/output.xlsx
@@ -415,9 +415,10 @@
         <v>H6838</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
 均碼 60 38 102 104 24 32
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="6" xml:space="preserve">
@@ -425,12 +426,13 @@
         <v>H6647</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 裙長 腰圍 臂圍 腳圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 裙長 腰圍 臂圍 腳圍
 S 33.5 64 90 62
 M 34.2 68 94 64
 L 34.9 72 98 66
 XL 35.6 76 102 68
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
@@ -438,9 +440,10 @@
         <v>H6844</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 後衣長 胸圍 擺轉 袖長 袖口
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 後衣長 胸圍 擺轉 袖長 袖口
 均碼 46 60 145 32 28
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="8" xml:space="preserve">
@@ -448,9 +451,10 @@
         <v>H6827</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
 均碼 70 37 112 114 22.5 35
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
@@ -458,9 +462,10 @@
         <v>H6839</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 後衣長 肩寬 胸圍 擺轉 袖長 袖口
 均碼 74 51 118 118 56 23
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="10" xml:space="preserve">
@@ -468,10 +473,11 @@
         <v>H6591</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 褲長 腰圍 臂轉 腿轉 膝轉 腳圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 褲長 腰圍 臂轉 腿轉 膝轉 腳圍
 S 92 64 100 65 56 52
 M 9 68 104 67.2 58 54
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="11" xml:space="preserve">
@@ -479,9 +485,10 @@
         <v>H6842</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 胸圍 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 胸圍 袖長
 均碼 72 55 112 20
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="12" xml:space="preserve">
@@ -489,9 +496,10 @@
         <v>H865</v>
       </c>
       <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 領軒 胸圍 下襬 夾直
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 領軒 胸圍 下襬 夾直
 均碼 57 22 44 45 47 16.5
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="13" xml:space="preserve">
@@ -499,9 +507,10 @@
         <v>H6819</v>
       </c>
       <c r="B13" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 肩寬 胸圍 擺轉 袖長 衣長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 肩寬 胸圍 擺轉 袖長 衣長
 均碼 47.5 108 110 21 70
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="14" xml:space="preserve">
@@ -509,12 +518,13 @@
         <v>H777</v>
       </c>
       <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 裙側長 腰圍 臂圍 腳圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 裙側長 腰圍 臂圍 腳圍
 S 39.5 64 87 94
 M 40.5 68 91 98
 L 41.5 72 95 102
 XL 42.5 76 99 106
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
@@ -522,9 +532,10 @@
         <v>H6881</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 胸圍 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 胸圍 袖長
 均碼 64 56 104 17.5
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="16" xml:space="preserve">
@@ -532,11 +543,12 @@
         <v>H6856</v>
       </c>
       <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 後衣長 ”後中長 胸圍 擺圍 腰圍 肩帶長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 後衣長 ”後中長 胸圍 擺圍 腰圍 肩帶長
 S 112 94 76 154 68 43
 M 113.5 95.5 80 158 72 43
 L 115 97 84 162 76 43
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="17" xml:space="preserve">
@@ -544,9 +556,10 @@
         <v>H6634</v>
       </c>
       <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 領國 胸圍 下襬 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 領國 胸圍 下襬 袖長
 均碼 85.5 38 58 102 114 28
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="18" xml:space="preserve">
@@ -554,12 +567,13 @@
         <v>H590</v>
       </c>
       <c r="B18" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 褲長 腰圍 臂圍 腿轉 膝轉 腳圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 褲長 腰圍 臂圍 腿轉 膝轉 腳圍
 S 103 64 90 59 52 44
 M 104 68 94 61.2 53.6 45.6
 L 105 72 98 63.4 55.2 47.2
 XL 106 76 102 65.6 56.8 48.8
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="19" xml:space="preserve">
@@ -567,9 +581,10 @@
         <v>H648</v>
       </c>
       <c r="B19" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 領軒 胸圍 下襬 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 領軒 胸圍 下襬 袖長
 均碼 63 58 58 116 118 63
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="20" xml:space="preserve">
@@ -577,12 +592,13 @@
         <v>H6624</v>
       </c>
       <c r="B20" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 裙長 腰圍 恬圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 裙長 腰圍 恬圍
 S 37.5 64 90
 M 38.5 68 94
 L 39.5 72 98
 XL 40.5 76 102
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="21" xml:space="preserve">
@@ -590,9 +606,10 @@
         <v>H6835</v>
       </c>
       <c r="B21" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 胸圍 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 胸圍 袖長
 均碼 71.5 53.5 108 22.5
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="22" xml:space="preserve">
@@ -600,9 +617,10 @@
         <v>H6872</v>
       </c>
       <c r="B22" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 胸圍 袖長 裙長 裙腰 祿擺
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 胸圍 袖長 裙長 裙腰 祿擺
 均碼 57 116 33 38.5 62 110
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="23" xml:space="preserve">
@@ -610,9 +628,10 @@
         <v>H6605</v>
       </c>
       <c r="B23" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 胸圍 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 胸圍 袖長
 均碼 54 87 31
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="24" xml:space="preserve">
@@ -620,12 +639,13 @@
         <v>H6603</v>
       </c>
       <c r="B24" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 “ 褲長 腰圍 氏圍 腿圍 腳圍 前浪 。 後浪
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 “ 褲長 腰圍 氏圍 腿圍 腳圍 前浪 。 後浪
 S 38 66 100 68 68 32 40.5
 M 38.7 70 104 70.2 70 32.6 41.3
 L 39.4 74 108 72.4 漢 332 42.1
 XL 40.1 78 再2 74.6 74 33.8 42.9
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="25" xml:space="preserve">
@@ -633,9 +653,10 @@
         <v>H6867</v>
       </c>
       <c r="B25" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 衣長 肩寬 胸圍 袖長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 衣長 肩寬 胸圍 袖長
 均碼 64 39.5 96 20.5
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="26" xml:space="preserve">
@@ -643,9 +664,10 @@
         <v>H6814</v>
       </c>
       <c r="B26" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼 肩寬 胸圍 擺轉 袖長 衣長
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼 肩寬 胸圍 擺轉 袖長 衣長
 均碼 43 100 102 19 60
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="27" xml:space="preserve">
@@ -653,9 +675,10 @@
         <v>H6883</v>
       </c>
       <c r="B27" t="str" xml:space="preserve">
-        <v xml:space="preserve">尺碼”衣長”户寬 前領口 後領口 胸圍 擺圍 前夾 ”前夾 ”腰圍
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺碼”衣長”户寬 前領口 後領口 胸圍 擺圍 前夾 ”前夾 ”腰圍
 均碼 。 117 32 46 60 73 164 21 21 62
-</v>
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refine size image logicla
</commit_message>
<xml_diff>
--- a/src/electron/crawler/config/output.xlsx
+++ b/src/electron/crawler/config/output.xlsx
@@ -397,12 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" t="str">
         <v>流水號</v>
       </c>
@@ -410,258 +414,511 @@
         <v>content</v>
       </c>
     </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>H6838</v>
-      </c>
-      <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 後衣長 60 肩寬 38 胸圍 102 擺轉 104 袖長 24 袖口 32
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6" t="str">
-        <v>H6647</v>
-      </c>
-      <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 裙長 33.5 腰圍 64 臂圍 90 腳圍 62
-尺碼 M 裙長 34.2 腰圍 68 臂圍 94 腳圍 64
-尺碼 L 裙長 34.9 腰圍 72 臂圍 98 腳圍 66
-尺碼 XL 裙長 35.6 腰圍 76 臂圍 102 腳圍 68
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="7" xml:space="preserve">
-      <c r="A7" t="str">
-        <v>H6844</v>
-      </c>
-      <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 後衣長 46 胸圍 60 擺轉 145 袖長 32 袖口 28
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="8" xml:space="preserve">
-      <c r="A8" t="str">
-        <v>H6827</v>
-      </c>
-      <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 後衣長 70 肩寬 37 胸圍 112 擺轉 114 袖長 22.5 袖口 35
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="9" xml:space="preserve">
-      <c r="A9" t="str">
-        <v>H6839</v>
-      </c>
-      <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 後衣長 74 肩寬 51 胸圍 118 擺轉 118 袖長 56 袖口 23
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
     <row r="10" xml:space="preserve">
       <c r="A10" t="str">
-        <v>H6591</v>
+        <v>F04418</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 褲長 92 腰圍 64 臂轉 100 腿轉 65 膝轉 56 腳圍 52
-尺碼 M 褲長 9 腰圍 68 臂轉 104 腿轉 67.2 膝轉 58 腳圍 54
+衣長45  胸圍74  袖長16
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="11" xml:space="preserve">
       <c r="A11" t="str">
-        <v>H6842</v>
+        <v>F04441</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 72 肩寬 55 胸圍 112 袖長 20
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="12" xml:space="preserve">
-      <c r="A12" t="str">
-        <v>H865</v>
-      </c>
-      <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 57 肩寬 22 領軒 44 胸圍 45 下襬 47 夾直 16.5
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="13" xml:space="preserve">
-      <c r="A13" t="str">
-        <v>H6819</v>
-      </c>
-      <c r="B13" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 肩寬 47.5 胸圍 108 擺轉 110 袖長 21 衣長 70
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="14" xml:space="preserve">
-      <c r="A14" t="str">
-        <v>H777</v>
-      </c>
-      <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 裙側長 39.5 腰圍 64 臂圍 87 腳圍 94
-尺碼 M 裙側長 40.5 腰圍 68 臂圍 91 腳圍 98
-尺碼 L 裙側長 41.5 腰圍 72 臂圍 95 腳圍 102
-尺碼 XL 裙側長 42.5 腰圍 76 臂圍 99 腳圍 106
+衣長46 肩寬33  胸圍86  袖長23
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
       <c r="A15" t="str">
-        <v>H6881</v>
+        <v>F04418</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 64 肩寬 56 胸圍 104 袖長 17.5
+衣長45  胸圍74  袖長16
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="16" xml:space="preserve">
       <c r="A16" t="str">
-        <v>H6856</v>
+        <v>F04441</v>
       </c>
       <c r="B16" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 後衣長 112 ”後中長 94 胸圍 76 擺圍 154 腰圍 68 肩帶長 43
-尺碼 M 後衣長 113.5 ”後中長 95.5 胸圍 80 擺圍 158 腰圍 72 肩帶長 43
-尺碼 L 後衣長 115 ”後中長 97 胸圍 84 擺圍 162 腰圍 76 肩帶長 43
+衣長46 肩寬33  胸圍86  袖長23
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="17" xml:space="preserve">
       <c r="A17" t="str">
-        <v>H6634</v>
+        <v>F04449</v>
       </c>
       <c r="B17" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 85.5 肩寬 38 領國 58 胸圍 102 下襬 114 袖長 28
+衣長47肩寬35袖長21胸圍98
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="18" xml:space="preserve">
       <c r="A18" t="str">
-        <v>H590</v>
+        <v>F04450</v>
       </c>
       <c r="B18" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 褲長 103 腰圍 64 臂圍 90 腿轉 59 膝轉 52 腳圍 44
-尺碼 M 褲長 104 腰圍 68 臂圍 94 腿轉 61.2 膝轉 53.6 腳圍 45.6
-尺碼 L 褲長 105 腰圍 72 臂圍 98 腿轉 63.4 膝轉 55.2 腳圍 47.2
-尺碼 XL 褲長 106 腰圍 76 臂圍 102 腿轉 65.6 膝轉 56.8 腳圍 48.8
+S碼:  衣長：42釐米 胸圍：70-92釐米（後背彈力）M碼: 衣長：43釐米 胸圍：74-96釐米（後背彈力）L碼:  衣長：44釐米 胸圍：78-100釐米（後背彈力）
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="19" xml:space="preserve">
       <c r="A19" t="str">
-        <v>H648</v>
+        <v>F04451</v>
       </c>
       <c r="B19" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 63 肩寬 58 領軒 58 胸圍 116 下襬 118 袖長 63
+尺才* S 肩寬、\ 39 胸圍\ 96 衣長， 58 袖長\ 24
+尺才* M 肩寬、\ 40 胸圍\ 100 衣長， 59 袖長\ 25
+尺才* L 肩寬、\ 41 胸圍\ 104 衣長， 60 袖長\ 26
+尺才* XL 肩寬、\ 42 胸圍\ 108 衣長， 61 袖長\ 27
+尺才* “由於測量方法不同，尺寸數據可能存在 肩寬、\ 1-4CM 胸圍\ 的誤差 衣長， undefined 袖長\ undefined
+尺才* 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長， S 袖長\ 寬鬆
+尺才* 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長， S 袖長\ 寬鬆
+尺才* 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長， M 袖長\ 合適
+尺才* 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長， S 袖長\ 寬鬆
+尺才* 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長， 上 袖長\ 修身
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="20" xml:space="preserve">
       <c r="A20" t="str">
-        <v>H6624</v>
+        <v>F04452</v>
       </c>
       <c r="B20" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S 裙長 37.5 腰圍 64 恬圍 90
-尺碼 M 裙長 38.5 腰圍 68 恬圍 94
-尺碼 L 裙長 39.5 腰圍 72 恬圍 98
-尺碼 XL 裙長 40.5 腰圍 76 恬圍 102
+尺寸\ S 衣長\、 61 胸圍\ 100 肩寬\ 37 袖長\ 25
+尺寸\ M 衣長\、 62 胸圍\ 104 肩寬\ 38 袖長\ 25.5
+尺寸\ L 衣長\、 63 胸圍\ 108 肩寬\ 39 袖長\ 26
+尺寸\ XL 衣長\、 64 胸圍\ 112 肩寬\ 40 袖長\ 26.5
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="21" xml:space="preserve">
       <c r="A21" t="str">
-        <v>H6835</v>
+        <v>F04453</v>
       </c>
       <c r="B21" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 71.5 肩寬 53.5 胸圍 108 袖長 22.5
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="22" xml:space="preserve">
-      <c r="A22" t="str">
-        <v>H6872</v>
-      </c>
-      <c r="B22" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 57 胸圍 116 袖長 33 裙長 38.5 裙腰 62 祿擺 110
+尺寸\ S 衣長\ 57 胸圍\ 92 肩寬\ 36 袖長\ 23
+尺寸\ M 衣長\ 58 胸圍\ 96 肩寬\ 37 袖長\ 23.5
+尺寸\ L 衣長\ 59 胸圍\ 100 肩寬\ 38 袖長\ 24
+尺寸\ XL 衣長\ 60 胸圍\ 104 肩寬\ 39 袖長\ 24.5
+尺寸\ XXL 衣長\ 61 胸圍\ 108 肩寬\ 40 袖長\ 25
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="23" xml:space="preserve">
       <c r="A23" t="str">
-        <v>H6605</v>
+        <v>F04401</v>
       </c>
       <c r="B23" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 54 胸圍 87 袖長 31
+尺寸\ S 肩寬、\ 39 胸圍\ 102 衣長\ 61 袖長\ 26
+尺寸\ M 肩寬、\ 40 胸圍\ 106 衣長\ 62 袖長\ 27
+尺寸\ L 肩寬、\ 41 胸圍\ 108 衣長\ 63 袖長\ 28
+尺寸\ XL 肩寬、\ 42 胸圍\ 112 衣長\ 64 袖長\ 29
+尺寸\ “由於測量方法不同，尺寸數據可能存在 肩寬、\ 1-4CM 胸圍\ 的誤差“ 衣長\ undefined 袖長\ undefined
+尺寸\ 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長\ M 袖長\ 合適
+尺寸\ 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長\ L 袖長\ 修身
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="24" xml:space="preserve">
       <c r="A24" t="str">
-        <v>H6603</v>
+        <v>F04402</v>
       </c>
       <c r="B24" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 S “ 38 褲長 66 腰圍 100 氏圍 68 腿圍 68 腳圍 32 前浪 40.5 。 undefined 後浪 undefined
-尺碼 M “ 38.7 褲長 70 腰圍 104 氏圍 70.2 腿圍 70 腳圍 32.6 前浪 41.3 。 undefined 後浪 undefined
-尺碼 L “ 39.4 褲長 74 腰圍 108 氏圍 72.4 腿圍 漢 腳圍 332 前浪 42.1 。 undefined 後浪 undefined
-尺碼 XL “ 40.1 褲長 78 腰圍 再2 氏圍 74.6 腿圍 74 腳圍 33.8 前浪 42.9 。 undefined 後浪 undefined
+尺寸\ S 肩寬、\ 39 胸圍\ 102 衣長\ 61 袖長\ 26
+尺寸\ M 肩寬、\ 40 胸圍\ 106 衣長\ 62 袖長\ 27
+尺寸\ L 肩寬、\ 41 胸圍\ 110 衣長\ 63 袖長\ 28
+尺寸\ XL 肩寬、\ 42 胸圍\ 114 衣長\ 64 袖長\ 29
+尺寸\ “由於測量方法不同，尺寸數據可能存在 肩寬、\ 1-4CM 胸圍\ 的誤差“ 衣長\ undefined 袖長\ undefined
+尺寸\ 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長\ M 袖長\ 合適
+尺寸\ 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長\ L 袖長\ 修身
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="25" xml:space="preserve">
       <c r="A25" t="str">
-        <v>H6867</v>
+        <v>F04403</v>
       </c>
       <c r="B25" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 衣長 64 肩寬 39.5 胸圍 96 袖長 20.5
-手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
-      </c>
-    </row>
-    <row r="26" xml:space="preserve">
-      <c r="A26" t="str">
-        <v>H6814</v>
-      </c>
-      <c r="B26" t="str" xml:space="preserve">
-        <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼 均碼 肩寬 43 胸圍 100 擺轉 102 袖長 19 衣長 60
+尺寸\ S 腰圍\ 64 臂圍\ 90 褲長\ 95
+尺寸\ M 腰圍\ 68 臂圍\ 93 褲長\ 96
+尺寸\ L 腰圍\ 72 臂圍\ 96 褲長\ 97
+尺寸\ XL 腰圍\ 76 臂圍\ 99 褲長\ 98
+尺寸\ “由於測量方法不同，尺十數據可能存在 腰圍\ 1-4CM 臂圍\ 的誤差“ 褲長\ undefined
+尺寸\ 小萌 腰圍\ 155cm 臂圍\ 40kg 褲長\ S
+尺寸\ 小琳 腰圍\ 158cm 臂圍\ 46kg 褲長\ 5
+尺寸\ 小妮 腰圍\ 163cm 臂圍\ 50kg 褲長\ M
+尺寸\ 小曹 腰圍\ 168cm 臂圍\ 45kg 褲長\ S
+尺寸\ 小琪 腰圍\ 169cm 臂圍\ 55kg 褲長\ 修身
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
     <row r="27" xml:space="preserve">
       <c r="A27" t="str">
-        <v>H6883</v>
+        <v>F04405</v>
       </c>
       <c r="B27" t="str" xml:space="preserve">
         <v xml:space="preserve">【尺 碼 信 息 x Size info】
-尺碼”衣長”户寬 均碼 前領口 。 後領口 117 胸圍 32 擺圍 46 前夾 60 ”前夾 73 ”腰圍 164
+尺寸\ S 肩寬、\ 59 胸圍\ 102 衣長\ 68 袖長\ 21
+尺寸\ M 肩寬、\ 60 胸圍\ 106 衣長\ 69 袖長\ 2
+尺寸\ L 肩寬、\ 61 胸圍\ 110 衣長\ 70 袖長\ 23
+尺寸\ XL 肩寬、\ 62 胸圍\ 114 衣長\ 71 袖長\ 24
+尺寸\ “由於測量方法不同，尺寸數據可能存在 肩寬、\ 1-4CM 胸圍\ 的誤差“ 衣長\ undefined 袖長\ undefined
+尺寸\ 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長\ M 袖長\ 合適
+尺寸\ 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長\ L 袖長\ 修身
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="29" xml:space="preserve">
+      <c r="A29" t="str">
+        <v>F04407</v>
+      </c>
+      <c r="B29" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺寸\ S 腰圍\ 60 臂圍\ 108 裙長\ 78
+尺寸\ M 腰圍\ 64 臂圍\ 112 裙長\ 79
+尺寸\ L 腰圍\ 68 臂圍\ 114 裙長\ 80
+尺寸\ XL 腰圍\ 72 臂圍\ 118 裙長\ 81
+尺寸\ “由於測量方法不同，尺十數據可能存在 腰圍\ 1-4CM 臂圍\ 的誤差“ 裙長\ undefined
+尺寸\ 小萌 腰圍\ 155cm 臂圍\ 40kg 裙長\ S
+尺寸\ 小琳 腰圍\ 158cm 臂圍\ 46kg 裙長\ S
+尺寸\ 小妮 腰圍\ 163cm 臂圍\ 50kg 裙長\ M
+尺寸\ 小鞋 腰圍\ 168cm 臂圍\ 45kg 裙長\ S
+尺寸\ 小琪 腰圍\ 169cm 臂圍\ 55kg 裙長\ 民
+尺寸\ 下瑟 腰圍\ 8S 臂圍\ undefined 裙長\ undefined
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="30" xml:space="preserve">
+      <c r="A30" t="str">
+        <v>F04408</v>
+      </c>
+      <c r="B30" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺寸\ S 肩寬、\ 60 胸圍\ 112 衣長\ 69 袖長\ 22
+尺寸\ M 肩寬、\ 61 胸圍\ 116 衣長\ 70 袖長\ 23
+尺寸\ L 肩寬、\ 62 胸圍\ 120 衣長\ 71 袖長\ 24
+尺寸\ X[L 肩寬、\ 63 胸圍\ 124 衣長\ 72 袖長\ 25
+尺寸\ * 肩寬、\ 由於測量方法不同，尺寸數據可能存在 胸圍\ 1-4CM 衣長\ 的誤差“* 袖長\ undefined
+尺寸\ 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長\ 交 袖長\ 寬鬆
+尺寸\ 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長\ M 袖長\ 合適
+尺寸\ 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長\ L 袖長\ 修身
+尺寸\ MODEL 肩寬、\ 3五 胸圍\ undefined 衣長\ undefined 袖長\ undefined
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="31" xml:space="preserve">
+      <c r="A31" t="str">
+        <v>F04409</v>
+      </c>
+      <c r="B31" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺寸 S 肩寬\ 32 胸圍、 位 腰圍 60 衣長\ 84 ， 25 袖長\ undefined
+尺寸 M 肩寬\ 33 胸圍、 6 腰圍 64 衣長\ 85 ， 26 袖長\ undefined
+尺寸 [L 肩寬\ 34 胸圍、 80 腰圍 68 衣長\ 86 ， 2 袖長\ undefined
+尺寸 XL 肩寬\ 35 胸圍、 84 腰圍 72 衣長\ 87 ， 28 袖長\ undefined
+尺寸 “由於測量方法不同，尺寸數據可能存在 肩寬\ 1-4CM 胸圍、 的誤差“ 腰圍 undefined 衣長\ undefined ， undefined 袖長\ undefined
+尺寸 小萌 肩寬\ 155cm 胸圍、 40kg 腰圍 S 衣長\ 寬鬆 ， undefined 袖長\ undefined
+尺寸 小琳 肩寬\ 158cm 胸圍、 46kg 腰圍 S 衣長\ 寬鬆 ， undefined 袖長\ undefined
+尺寸 小妮 肩寬\ 163cm 胸圍、 50kg 腰圍 M 衣長\ 合適 ， undefined 袖長\ undefined
+尺寸 小曹 肩寬\ 168cm 胸圍、 45kg 腰圍 S 衣長\ 寬鬆 ， undefined 袖長\ undefined
+尺寸 小琪 肩寬\ 169cm 胸圍、 55kg 腰圍 修身 衣長\ undefined ， undefined 袖長\ undefined
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="32" xml:space="preserve">
+      <c r="A32" t="str">
+        <v>F04410</v>
+      </c>
+      <c r="B32" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+尺寸\ S 肩寬、\ 32 胸圍\ 102 衣長\ 51 袖長\ 26
+尺寸\ M 肩寬、\ 33 胸圍\ 106 衣長\ 52 袖長\ 27
+尺寸\ L 肩寬、\ 34 胸圍\ 110 衣長\ 53 袖長\ 28
+尺寸\ X[L 肩寬、\ 35 胸圍\ 114 衣長\ 54 袖長\ 29
+尺寸\ * 肩寬、\ 由於測量方法不同，尺寸數據可能存在 胸圍\ 1-4CM 衣長\ 的誤差“* 袖長\ undefined
+尺寸\ 小萌 肩寬、\ 155cm 胸圍\ 40kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琳 肩寬、\ 158cm 胸圍\ 46kg 衣長\ 交 袖長\ 寬鬆
+尺寸\ 小妮 肩寬、\ 163cm 胸圍\ 50kg 衣長\ M 袖長\ 合適
+尺寸\ 小曹 肩寬、\ 168cm 胸圍\ 45kg 衣長\ S 袖長\ 寬鬆
+尺寸\ 小琪 肩寬、\ 169cm 胸圍\ 55kg 衣長\ L 袖長\ 修身
+尺寸\ MODEL 肩寬、\ 3五 胸圍\ undefined 衣長\ undefined 袖長\ undefined
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="34" xml:space="preserve">
+      <c r="A34" t="str">
+        <v>F04414</v>
+      </c>
+      <c r="B34" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長49 胸圍82 袖長23
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="38" xml:space="preserve">
+      <c r="A38" t="str">
+        <v>F04421</v>
+      </c>
+      <c r="B38" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+S 衣長80  腰圍56M 衣長81  腰圍60L 衣長82  腰圍64XL 衣長83  腰圍68
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="40" xml:space="preserve">
+      <c r="A40" t="str">
+        <v>F04423</v>
+      </c>
+      <c r="B40" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+胸圍96 全長44
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="41" xml:space="preserve">
+      <c r="A41" t="str">
+        <v>F04425</v>
+      </c>
+      <c r="B41" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+肩寬28 胸圍49 袖長21 全長113
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="45" xml:space="preserve">
+      <c r="A45" t="str">
+        <v>F04430</v>
+      </c>
+      <c r="B45" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+吊帶 衣長39 胸圍84
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="46" xml:space="preserve">
+      <c r="A46" t="str">
+        <v>F04430</v>
+      </c>
+      <c r="B46" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+半身裙 裙長82 腰圍64
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="48" xml:space="preserve">
+      <c r="A48" t="str">
+        <v>F04432</v>
+      </c>
+      <c r="B48" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+裙長：119cm 胸圍：112cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="49" xml:space="preserve">
+      <c r="A49" t="str">
+        <v>F04433</v>
+      </c>
+      <c r="B49" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長：37cm 胸圍：64-98cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="50" xml:space="preserve">
+      <c r="A50" t="str">
+        <v>F04434</v>
+      </c>
+      <c r="B50" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+ 衣長：48cm  胸圍：62-98cm 肩寬：35cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="51" xml:space="preserve">
+      <c r="A51" t="str">
+        <v>F04435</v>
+      </c>
+      <c r="B51" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+ 衣長：36cm  胸圍：58-92cm  袖長：22cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="52" xml:space="preserve">
+      <c r="A52" t="str">
+        <v>F04436</v>
+      </c>
+      <c r="B52" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+上衣 衣長：45cm 胸圍：76-118cm （可拉伸 ）肩寬：31cm 袖長：18cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="53" xml:space="preserve">
+      <c r="A53" t="str">
+        <v>F04436</v>
+      </c>
+      <c r="B53" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+褲子 褲長：89cm 腰圍：56cm 大腿圍：68cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="54" xml:space="preserve">
+      <c r="A54" t="str">
+        <v>F04437</v>
+      </c>
+      <c r="B54" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長：42cm 胸圍：64-98cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="55" xml:space="preserve">
+      <c r="A55" t="str">
+        <v>F04438</v>
+      </c>
+      <c r="B55" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長：44cm 胸圍：60-96cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="56" xml:space="preserve">
+      <c r="A56" t="str">
+        <v>F04439</v>
+      </c>
+      <c r="B56" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長：52cm 胸圍：68-102cm 袖長：17cm
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="57" xml:space="preserve">
+      <c r="A57" t="str">
+        <v>F04440</v>
+      </c>
+      <c r="B57" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+ 衣長：43cm 胸圍：62-98cm 
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="58" xml:space="preserve">
+      <c r="A58" t="str">
+        <v>F04442</v>
+      </c>
+      <c r="B58" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長48 胸圍92 肩寬33 袖長22 （上衣不分尺碼）
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="59" xml:space="preserve">
+      <c r="A59" t="str">
+        <v>F04442</v>
+      </c>
+      <c r="B59" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+半身裙S碼 裙長85 腰圍64
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="60" xml:space="preserve">
+      <c r="A60" t="str">
+        <v>F04442</v>
+      </c>
+      <c r="B60" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+M碼 裙長86 腰圍68
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="61" xml:space="preserve">
+      <c r="A61" t="str">
+        <v>F04443</v>
+      </c>
+      <c r="B61" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+裙長112 肩寬31 胸圍76 袖長25
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="62" xml:space="preserve">
+      <c r="A62" t="str">
+        <v>F04444</v>
+      </c>
+      <c r="B62" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+裙長118 胸圍88 袖長45
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="63" xml:space="preserve">
+      <c r="A63" t="str">
+        <v>F04445</v>
+      </c>
+      <c r="B63" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+裙長113 胸圍86
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="64" xml:space="preserve">
+      <c r="A64" t="str">
+        <v>F04446</v>
+      </c>
+      <c r="B64" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+衣長52 肩寬35 胸圍94 袖長23
+手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
+      </c>
+    </row>
+    <row r="66" xml:space="preserve">
+      <c r="A66" t="str">
+        <v>F04448</v>
+      </c>
+      <c r="B66" t="str" xml:space="preserve">
+        <v xml:space="preserve">【尺 碼 信 息 x Size info】
+胸圍：70-100 衣長：45          
 手工平鋪測量，誤差允許在2~5cm左右，具體以實物為準</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O66"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>